<commit_message>
adicionado cooldown e modelo de banco de dados
</commit_message>
<xml_diff>
--- a/pokemon.xlsx
+++ b/pokemon.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="186">
   <si>
     <t>BULBASAUR</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>120S</t>
+  </si>
+  <si>
+    <t>Water</t>
   </si>
 </sst>
 </file>
@@ -929,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -942,7 +945,7 @@
     <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +962,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -976,7 +979,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -993,7 +996,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1060,8 +1063,14 @@
       <c r="E7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1078,7 +1087,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1095,7 +1104,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1112,7 +1121,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1129,7 +1138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1146,7 +1155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1163,7 +1172,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1180,7 +1189,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1197,7 +1206,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
correcoes feitas no CharacterSelect
</commit_message>
<xml_diff>
--- a/pokemon.xlsx
+++ b/pokemon.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="191">
   <si>
     <t>BULBASAUR</t>
   </si>
@@ -590,6 +590,21 @@
   </si>
   <si>
     <t>Water</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Bug/Flying</t>
+  </si>
+  <si>
+    <t>Normal/Flying</t>
+  </si>
+  <si>
+    <t>Thunder Stone</t>
+  </si>
+  <si>
+    <t>Fire/Flying</t>
   </si>
 </sst>
 </file>
@@ -932,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -961,6 +976,12 @@
       <c r="E1" t="s">
         <v>54</v>
       </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
@@ -978,6 +999,12 @@
       <c r="E2" t="s">
         <v>56</v>
       </c>
+      <c r="F2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
@@ -995,6 +1022,9 @@
       <c r="E3" t="s">
         <v>58</v>
       </c>
+      <c r="F3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
@@ -1012,6 +1042,12 @@
       <c r="E4" t="s">
         <v>60</v>
       </c>
+      <c r="F4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -1029,6 +1065,12 @@
       <c r="E5" t="s">
         <v>62</v>
       </c>
+      <c r="F5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
@@ -1046,6 +1088,9 @@
       <c r="E6" t="s">
         <v>64</v>
       </c>
+      <c r="F6" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
@@ -1086,6 +1131,12 @@
       <c r="E8" t="s">
         <v>67</v>
       </c>
+      <c r="F8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
@@ -1103,6 +1154,9 @@
       <c r="E9" t="s">
         <v>68</v>
       </c>
+      <c r="F9" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
@@ -1120,6 +1174,12 @@
       <c r="E10" t="s">
         <v>54</v>
       </c>
+      <c r="F10" t="s">
+        <v>186</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
@@ -1137,6 +1197,12 @@
       <c r="E11" t="s">
         <v>69</v>
       </c>
+      <c r="F11" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
@@ -1154,6 +1220,9 @@
       <c r="E12" t="s">
         <v>56</v>
       </c>
+      <c r="F12" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
@@ -1171,6 +1240,12 @@
       <c r="E13" t="s">
         <v>72</v>
       </c>
+      <c r="F13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -1188,6 +1263,12 @@
       <c r="E14" t="s">
         <v>54</v>
       </c>
+      <c r="F14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
@@ -1205,6 +1286,9 @@
       <c r="E15" t="s">
         <v>77</v>
       </c>
+      <c r="F15" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
@@ -1222,6 +1306,12 @@
       <c r="E16" t="s">
         <v>72</v>
       </c>
+      <c r="F16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G16">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
@@ -1239,6 +1329,12 @@
       <c r="E17" t="s">
         <v>78</v>
       </c>
+      <c r="F17" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
@@ -1256,6 +1352,9 @@
       <c r="E18" t="s">
         <v>80</v>
       </c>
+      <c r="F18" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
@@ -1273,6 +1372,12 @@
       <c r="E19" t="s">
         <v>85</v>
       </c>
+      <c r="F19" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
@@ -1290,6 +1395,9 @@
       <c r="E20" t="s">
         <v>89</v>
       </c>
+      <c r="F20" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
@@ -1307,6 +1415,12 @@
       <c r="E21" t="s">
         <v>72</v>
       </c>
+      <c r="F21" t="s">
+        <v>188</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
@@ -1324,6 +1438,9 @@
       <c r="E22" t="s">
         <v>77</v>
       </c>
+      <c r="F22" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
@@ -1341,6 +1458,12 @@
       <c r="E23" t="s">
         <v>97</v>
       </c>
+      <c r="F23" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
@@ -1358,6 +1481,9 @@
       <c r="E24" t="s">
         <v>56</v>
       </c>
+      <c r="F24" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
@@ -1374,6 +1500,12 @@
       </c>
       <c r="E25" t="s">
         <v>97</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:7">

</xml_diff>